<commit_message>
Update budget plots and fit search
</commit_message>
<xml_diff>
--- a/Outputs/1. Budget/Grid Search/Evaluation Metrics.xlsx
+++ b/Outputs/1. Budget/Grid Search/Evaluation Metrics.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/microgrid_MP/Outputs/1. Budget/Grid Search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_59D5E13DDA30921FD2FE31D2F8F2D3C2D4D9039E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F5A084F-B81A-4B1D-84E9-D6D25A5CA875}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_085DE507547F320F6235547658A166788E558665" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BED82460-7FE7-412D-A623-769D8B22A7EF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Budget</t>
+  </si>
   <si>
     <t>FiT</t>
   </si>
@@ -39,9 +42,6 @@
   <si>
     <t>Wasted generation (from total)</t>
   </si>
-  <si>
-    <t>Budget</t>
-  </si>
 </sst>
 </file>
 
@@ -58,10 +58,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,9 +119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -162,7 +159,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -196,7 +193,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -231,10 +227,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -411,36 +406,36 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -454,16 +449,16 @@
         <v>0.4</v>
       </c>
       <c r="D2">
-        <v>0.35836827204850769</v>
+        <v>0.35818875238055309</v>
       </c>
       <c r="E2">
-        <v>0.22348028102234541</v>
+        <v>0.22197198218901401</v>
       </c>
       <c r="F2">
-        <v>5700859.5294516822</v>
+        <v>5704260.7247040588</v>
       </c>
       <c r="G2">
-        <v>0.13145055786183099</v>
+        <v>0.1305633801557857</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -471,22 +466,22 @@
         <v>250000</v>
       </c>
       <c r="B3">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="C3">
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
       <c r="D3">
-        <v>0.14490559857105051</v>
+        <v>0.17682660770120409</v>
       </c>
       <c r="E3">
-        <v>0.12916507200038191</v>
+        <v>0.1217739969044872</v>
       </c>
       <c r="F3">
-        <v>7926212.885027498</v>
+        <v>7719893.0520599103</v>
       </c>
       <c r="G3">
-        <v>7.5974581260778412E-2</v>
+        <v>7.1627168862201274E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -494,22 +489,22 @@
         <v>400000</v>
       </c>
       <c r="B4">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="C4">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
       <c r="D4">
-        <v>0.1242994405177532</v>
+        <v>0.12881565437962009</v>
       </c>
       <c r="E4">
-        <v>9.7284084894617373E-2</v>
+        <v>0.1086785250784499</v>
       </c>
       <c r="F4">
-        <v>8360841.2282423368</v>
+        <v>8203619.0975476587</v>
       </c>
       <c r="G4">
-        <v>5.7222262169951917E-2</v>
+        <v>6.392444417829786E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -517,22 +512,22 @@
         <v>750000</v>
       </c>
       <c r="B5">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C5">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
       <c r="D5">
-        <v>2.881684065337459E-2</v>
+        <v>2.651314960383595E-2</v>
       </c>
       <c r="E5">
-        <v>0.1023872458912847</v>
+        <v>9.3559321760570274E-2</v>
       </c>
       <c r="F5">
-        <v>9520175.7428226136</v>
+        <v>9259228.2585114501</v>
       </c>
       <c r="G5">
-        <v>6.0223929058869009E-2</v>
+        <v>5.5031365551987163E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -540,19 +535,19 @@
         <v>1000000</v>
       </c>
       <c r="B6">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="C6">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D6">
         <v>3.7984572108003253E-2</v>
       </c>
       <c r="E6">
-        <v>0.17411554944671309</v>
+        <v>0.17411554944671301</v>
       </c>
       <c r="F6">
-        <v>9675252.0044199117</v>
+        <v>9817522.7338737287</v>
       </c>
       <c r="G6">
         <v>0.1024143427889334</v>
@@ -563,22 +558,22 @@
         <v>1250000</v>
       </c>
       <c r="B7">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="C7">
-        <v>0.28999999999999998</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D7">
         <v>3.7984572108003288E-2</v>
       </c>
       <c r="E7">
-        <v>0.16804243886007611</v>
+        <v>0.1680424388600758</v>
       </c>
       <c r="F7">
-        <v>9734124.3429999948</v>
+        <v>9875590.1982903536</v>
       </c>
       <c r="G7">
-        <v>9.8842153909816169E-2</v>
+        <v>9.8842153909815988E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -586,22 +581,22 @@
         <v>1500000</v>
       </c>
       <c r="B8">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="C8">
-        <v>0.28999999999999998</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D8">
         <v>3.7984572108003323E-2</v>
       </c>
       <c r="E8">
-        <v>0.1680424388600755</v>
+        <v>0.168042438860076</v>
       </c>
       <c r="F8">
-        <v>9734124.3429999929</v>
+        <v>9875590.1982903536</v>
       </c>
       <c r="G8">
-        <v>9.8842153909815822E-2</v>
+        <v>9.8842153909816127E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -609,22 +604,22 @@
         <v>1750000</v>
       </c>
       <c r="B9">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="C9">
-        <v>0.28999999999999998</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D9">
-        <v>3.7984572108003288E-2</v>
+        <v>3.7984572108003253E-2</v>
       </c>
       <c r="E9">
-        <v>0.16804243886007611</v>
+        <v>0.16804243886007619</v>
       </c>
       <c r="F9">
-        <v>9734124.3429999948</v>
+        <v>9875590.1982903555</v>
       </c>
       <c r="G9">
-        <v>9.8842153909816169E-2</v>
+        <v>9.8842153909816211E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -632,25 +627,25 @@
         <v>2000000</v>
       </c>
       <c r="B10">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="C10">
-        <v>0.28999999999999998</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D10">
-        <v>3.7984572108003288E-2</v>
+        <v>3.7984572108003253E-2</v>
       </c>
       <c r="E10">
         <v>0.16804243886007611</v>
       </c>
       <c r="F10">
-        <v>9734124.3429999948</v>
+        <v>9875590.1982903536</v>
       </c>
       <c r="G10">
         <v>9.8842153909816169E-2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>